<commit_message>
Tenant and service path in frontend tables
</commit_message>
<xml_diff>
--- a/StarSeeker/operator/samples/category.xlsx
+++ b/StarSeeker/operator/samples/category.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\yuta\work\StarSeeker\StarSeeker\operator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E997DA-9C9C-4B23-BC3A-47DC84361486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C686237E-36E7-4F67-B0CA-5BC5520BEC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>公共施設</t>
     <rPh sb="0" eb="4">
@@ -102,6 +102,25 @@
   </si>
   <si>
     <t>#カテゴリID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#テナント名</t>
+    <rPh sb="5" eb="6">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sample_government_plan</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sample_flood_control</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sample_public_facility</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -466,18 +485,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB64F55-DEA2-416E-92FA-60CC0F3630E2}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" customWidth="1"/>
+    <col min="3" max="3" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -485,16 +506,19 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -502,16 +526,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -519,16 +546,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -536,12 +566,15 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create and delete data in postgres and orion
</commit_message>
<xml_diff>
--- a/StarSeeker/operator/samples/category.xlsx
+++ b/StarSeeker/operator/samples/category.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\yuta\work\StarSeeker\StarSeeker\operator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C686237E-36E7-4F67-B0CA-5BC5520BEC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F6020E-59CE-4688-BBBD-717EC2EA1274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>公共施設</t>
     <rPh sb="0" eb="4">
@@ -43,13 +43,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>政策区域</t>
-    <rPh sb="0" eb="4">
-      <t>セイサククイキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>水域情報</t>
     <rPh sb="0" eb="4">
       <t>スイイキジョウホウ</t>
@@ -61,10 +54,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>#800000</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>#65ace4</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -105,22 +94,26 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>#テナント名</t>
-    <rPh sb="5" eb="6">
+    <t>テナント名</t>
+    <rPh sb="4" eb="5">
       <t>メイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>sample_government_plan</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sample_flood_control</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sample_public_facility</t>
+    <t>112399_sakado_city</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/public_facility</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/flood_control</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サービスパス</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -485,40 +478,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB64F55-DEA2-416E-92FA-60CC0F3630E2}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.3984375" customWidth="1"/>
-    <col min="3" max="3" width="31.19921875" customWidth="1"/>
+    <col min="3" max="4" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -526,56 +522,42 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3">
         <v>3</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
+      <c r="G3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More simple table structures and sample csv formats: auto serial id and constraint (unique and foreign keys cascade deleting)
</commit_message>
<xml_diff>
--- a/StarSeeker/operator/samples/category.xlsx
+++ b/StarSeeker/operator/samples/category.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\yuta\work\StarSeeker\StarSeeker\operator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F6020E-59CE-4688-BBBD-717EC2EA1274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E81288-7F25-49F4-BF87-5EB62787C1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>公共施設</t>
     <rPh sb="0" eb="4">
@@ -72,13 +72,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>カテゴリ名</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>有効</t>
     <rPh sb="0" eb="2">
       <t>ユウコウ</t>
@@ -90,30 +83,34 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>#カテゴリID</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テナント名</t>
-    <rPh sb="4" eb="5">
+    <t>112399_sakado_city</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/public_facility</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/flood_control</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サービスパス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#カテゴリ名</t>
+    <rPh sb="5" eb="6">
       <t>メイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>112399_sakado_city</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/public_facility</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/flood_control</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>サービスパス</t>
+    <t>テナント</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>112399_sakado_city_flood_control</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -478,86 +475,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB64F55-DEA2-416E-92FA-60CC0F3630E2}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" customWidth="1"/>
-    <col min="3" max="4" width="31.19921875" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" customWidth="1"/>
+    <col min="2" max="3" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backend support of fiware-* headers
</commit_message>
<xml_diff>
--- a/StarSeeker/operator/samples/category.xlsx
+++ b/StarSeeker/operator/samples/category.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\yuta\work\StarSeeker\StarSeeker\operator\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\yuta\work\StarSeeker\StarSeeker\operator\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E81288-7F25-49F4-BF87-5EB62787C1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EAE4CA-68C8-48C5-8EF0-256512E6E3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>公共施設</t>
     <rPh sb="0" eb="4">
@@ -111,6 +111,47 @@
   </si>
   <si>
     <t>112399_sakado_city_flood_control</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>施設サンプル</t>
+    <rPh sb="0" eb="2">
+      <t>シセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NULL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NULL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#1f1f1f</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>地域施設サンプル</t>
+    <rPh sb="0" eb="2">
+      <t>チイキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サンプル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#1f0000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#1f1f00</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -475,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB64F55-DEA2-416E-92FA-60CC0F3630E2}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -509,16 +550,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -529,21 +570,81 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: dataset selection without category
</commit_message>
<xml_diff>
--- a/StarSeeker/operator/samples/category.xlsx
+++ b/StarSeeker/operator/samples/category.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\yuta\work\StarSeeker\StarSeeker\operator\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBBBC56-5D0B-481A-B730-C204D3C9BF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B556C04-95F0-42ED-B47A-E24A32F8BD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>水域情報</t>
     <rPh sb="0" eb="4">
@@ -105,6 +105,26 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t>シセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>行政施設</t>
+    <rPh sb="0" eb="2">
+      <t>ギョウセイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>行政区域</t>
+    <rPh sb="0" eb="2">
+      <t>ギョウセイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>クイキ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -470,17 +490,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB64F55-DEA2-416E-92FA-60CC0F3630E2}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="3" width="31.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -500,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -520,23 +542,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E5">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sample data with tenant and service path
</commit_message>
<xml_diff>
--- a/StarSeeker/operator/samples/category.xlsx
+++ b/StarSeeker/operator/samples/category.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\home\yuta\work\StarSeeker\StarSeeker\operator\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\yuta\work\StarSeeker\StarSeeker\operator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B556C04-95F0-42ED-B47A-E24A32F8BD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EC3C90-20AA-4A70-9ADE-9B032EACDABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
+    <workbookView xWindow="7240" yWindow="2110" windowWidth="12260" windowHeight="7890" tabRatio="524" xr2:uid="{03898D4D-7442-4456-BE0F-5576AA6ABBF9}"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>水域情報</t>
     <rPh sb="0" eb="4">
@@ -126,6 +126,44 @@
     <rPh sb="2" eb="4">
       <t>クイキ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>government</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>公園</t>
+    <rPh sb="0" eb="2">
+      <t>コウエン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/park</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#001f00</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#00001f</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#fc4922</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>観光</t>
+    <rPh sb="0" eb="2">
+      <t>カンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/inbound</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -490,11 +528,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB64F55-DEA2-416E-92FA-60CC0F3630E2}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -536,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -547,13 +583,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -567,16 +603,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -584,21 +620,61 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>